<commit_message>
Act Tablas CENSO 2018 GT
</commit_message>
<xml_diff>
--- a/Guatemala/CENSO 2018/Cuadro A3 - Población de 10 años y más por estado conyugal.xlsx
+++ b/Guatemala/CENSO 2018/Cuadro A3 - Población de 10 años y más por estado conyugal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Comunicaciones REDD Dropbox\Patricio Emanuelli\0000 DOCUMENTACIÓN REDD+ Guatemala\MRV_REDD_Guatemala\BD_GT\CENSO 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-MUNI\Guatemala\CENSO 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B832BF7B-5A3C-41A9-A637-6C0BA926FDFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8647AE-2177-48AA-8033-ECA94CC0D7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A3_1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,26 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">A3_1!$1:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">A3_2!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="360">
   <si>
     <t>Características generales de la población. Censo 2018</t>
   </si>
@@ -1109,25 +1118,7 @@
     <t>Quesada</t>
   </si>
   <si>
-    <t>Estado conyugal: Soltera(o)</t>
-  </si>
-  <si>
     <t>Código2</t>
-  </si>
-  <si>
-    <t>Estado conyugal: Soltera(o)3</t>
-  </si>
-  <si>
-    <t>Estado conyugal: Soltera(o)4</t>
-  </si>
-  <si>
-    <t>Estado conyugal: Soltera(o)5</t>
-  </si>
-  <si>
-    <t>Estado conyugal: Soltera(o)6</t>
-  </si>
-  <si>
-    <t>Estado conyugal: Soltera(o)7</t>
   </si>
 </sst>
 </file>
@@ -1340,15 +1331,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1364,62 +1346,21 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1814,6 +1755,56 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1828,20 +1819,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DA71F41-CBC9-4EF1-BD89-B80AFD90AC6F}" name="Estado_Conyugal" displayName="Estado_Conyugal" ref="A4:K344" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DA71F41-CBC9-4EF1-BD89-B80AFD90AC6F}" name="Estado_Conyugal" displayName="Estado_Conyugal" ref="A4:K344" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A4:K344" xr:uid="{FD5C9A95-7DE4-4BB0-9BEB-06BB5CD9947C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9662113E-77F4-421D-957C-9747DE0BFE02}" name="Código" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{C4377192-7CFB-4DB0-93A9-9EAC41F235EC}" name="Departamento" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{49512B1A-4D24-4FDA-AF3F-F9893DC1B92B}" name="Código2" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{6EBD0CBF-1ED3-4C9A-9BCB-CA7F62A8257A}" name="Municipio" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{445F4005-52D5-4512-A5B6-7B4CEA8E8B63}" name="Población de 10 años y más" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{9A2DA39A-F466-4095-A3CA-487501EA738D}" name="Estado conyugal: Soltera(o)" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{8B948116-460B-4C7A-A756-55DFBF20B87B}" name="Estado conyugal: Soltera(o)3" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{479395F4-9475-4F25-AC31-E362254E3404}" name="Estado conyugal: Soltera(o)4" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{1632D080-83DC-4CC7-8ABB-33C0597686A7}" name="Estado conyugal: Soltera(o)5" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{244E81D5-E31E-4C1C-A974-35DFB00BA9DA}" name="Estado conyugal: Soltera(o)6" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{E1FCBF89-D041-45D1-A30D-823EB5CE8FCA}" name="Estado conyugal: Soltera(o)7" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9662113E-77F4-421D-957C-9747DE0BFE02}" name="Código" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{C4377192-7CFB-4DB0-93A9-9EAC41F235EC}" name="Departamento" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{49512B1A-4D24-4FDA-AF3F-F9893DC1B92B}" name="Código2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{6EBD0CBF-1ED3-4C9A-9BCB-CA7F62A8257A}" name="Municipio" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{445F4005-52D5-4512-A5B6-7B4CEA8E8B63}" name="Población de 10 años y más" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{9A2DA39A-F466-4095-A3CA-487501EA738D}" name="Soltera(o)" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{8B948116-460B-4C7A-A756-55DFBF20B87B}" name="Unida(o)" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{479395F4-9475-4F25-AC31-E362254E3404}" name="Casada(o)" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1632D080-83DC-4CC7-8ABB-33C0597686A7}" name="Separada(o)" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{244E81D5-E31E-4C1C-A974-35DFB00BA9DA}" name="Divorciada(o)" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{E1FCBF89-D041-45D1-A30D-823EB5CE8FCA}" name="Viuda(o)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2116,56 +2107,56 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D6" sqref="D6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="11"/>
-    <col min="7" max="7" width="17.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="10.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.44140625" style="11"/>
+    <col min="7" max="7" width="17.109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="5" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+    </row>
+    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2185,7 +2176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
@@ -2208,7 +2199,7 @@
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="12" t="s">
         <v>12</v>
@@ -2241,8 +2232,8 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" spans="1:21" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2271,7 +2262,7 @@
         <v>98236</v>
       </c>
     </row>
-    <row r="11" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>2</v>
       </c>
@@ -2300,7 +2291,7 @@
         <v>6099</v>
       </c>
     </row>
-    <row r="12" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>3</v>
       </c>
@@ -2329,7 +2320,7 @@
         <v>9548</v>
       </c>
     </row>
-    <row r="13" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>4</v>
       </c>
@@ -2358,7 +2349,7 @@
         <v>17761</v>
       </c>
     </row>
-    <row r="14" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>5</v>
       </c>
@@ -2387,7 +2378,7 @@
         <v>22601</v>
       </c>
     </row>
-    <row r="15" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>6</v>
       </c>
@@ -2416,7 +2407,7 @@
         <v>12741</v>
       </c>
     </row>
-    <row r="16" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>7</v>
       </c>
@@ -2445,7 +2436,7 @@
         <v>12048</v>
       </c>
     </row>
-    <row r="17" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>8</v>
       </c>
@@ -2474,7 +2465,7 @@
         <v>13660</v>
       </c>
     </row>
-    <row r="18" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>9</v>
       </c>
@@ -2503,7 +2494,7 @@
         <v>26182</v>
       </c>
     </row>
-    <row r="19" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>10</v>
       </c>
@@ -2532,7 +2523,7 @@
         <v>18350</v>
       </c>
     </row>
-    <row r="20" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>11</v>
       </c>
@@ -2561,7 +2552,7 @@
         <v>11272</v>
       </c>
     </row>
-    <row r="21" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>12</v>
       </c>
@@ -2590,7 +2581,7 @@
         <v>29748</v>
       </c>
     </row>
-    <row r="22" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>13</v>
       </c>
@@ -2619,7 +2610,7 @@
         <v>27285</v>
       </c>
     </row>
-    <row r="23" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>14</v>
       </c>
@@ -2648,7 +2639,7 @@
         <v>25419</v>
       </c>
     </row>
-    <row r="24" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>15</v>
       </c>
@@ -2677,7 +2668,7 @@
         <v>8249</v>
       </c>
     </row>
-    <row r="25" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>16</v>
       </c>
@@ -2706,7 +2697,7 @@
         <v>24375</v>
       </c>
     </row>
-    <row r="26" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>17</v>
       </c>
@@ -2735,7 +2726,7 @@
         <v>11704</v>
       </c>
     </row>
-    <row r="27" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>18</v>
       </c>
@@ -2764,7 +2755,7 @@
         <v>11239</v>
       </c>
     </row>
-    <row r="28" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>19</v>
       </c>
@@ -2793,7 +2784,7 @@
         <v>8412</v>
       </c>
     </row>
-    <row r="29" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>20</v>
       </c>
@@ -2827,7 +2818,7 @@
       <c r="T29" s="16"/>
       <c r="U29" s="16"/>
     </row>
-    <row r="30" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>21</v>
       </c>
@@ -2861,7 +2852,7 @@
       <c r="T30" s="16"/>
       <c r="U30" s="16"/>
     </row>
-    <row r="31" spans="1:28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>22</v>
       </c>
@@ -2902,7 +2893,7 @@
       <c r="T31" s="16"/>
       <c r="U31" s="16"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
@@ -2932,7 +2923,7 @@
       <c r="AA32" s="24"/>
       <c r="AB32" s="24"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>35</v>
       </c>
@@ -2947,7 +2938,7 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
@@ -2958,7 +2949,7 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="24"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
@@ -2969,7 +2960,7 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="24"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
@@ -3005,23 +2996,27 @@
   </sheetPr>
   <dimension ref="A1:Q346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N341" sqref="N341"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="31" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="29" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="11" customWidth="1"/>
-    <col min="7" max="11" width="28.42578125" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="10.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3030,49 +3025,49 @@
       <c r="D1" s="5"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="27"/>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="39" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>359</v>
+        <v>6</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>361</v>
+        <v>7</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>362</v>
+        <v>8</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>363</v>
+        <v>9</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>364</v>
+        <v>10</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -3107,7 +3102,7 @@
         <v>36775</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -3142,7 +3137,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -3177,7 +3172,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -3212,7 +3207,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>1</v>
       </c>
@@ -3282,7 +3277,7 @@
         <v>3547</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>1</v>
       </c>
@@ -3317,7 +3312,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>1</v>
       </c>
@@ -3352,7 +3347,7 @@
         <v>16119</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>1</v>
       </c>
@@ -3387,7 +3382,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -3422,7 +3417,7 @@
         <v>5758</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>1</v>
       </c>
@@ -3457,7 +3452,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -3492,7 +3487,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>1</v>
       </c>
@@ -3527,7 +3522,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>3291</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>1</v>
       </c>
@@ -3597,7 +3592,7 @@
         <v>13080</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1</v>
       </c>
@@ -3632,7 +3627,7 @@
         <v>4035</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>1</v>
       </c>
@@ -3667,7 +3662,7 @@
         <v>3627</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>2</v>
       </c>
@@ -3702,7 +3697,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>2</v>
       </c>
@@ -3737,7 +3732,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>2</v>
       </c>
@@ -3772,7 +3767,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>2</v>
       </c>
@@ -3807,7 +3802,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>2</v>
       </c>
@@ -3842,7 +3837,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>2</v>
       </c>
@@ -3877,7 +3872,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>2</v>
       </c>
@@ -3912,7 +3907,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>2</v>
       </c>
@@ -3947,7 +3942,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>3</v>
       </c>
@@ -3982,7 +3977,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>3</v>
       </c>
@@ -4017,7 +4012,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>3</v>
       </c>
@@ -4052,7 +4047,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>3</v>
       </c>
@@ -4087,7 +4082,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>3</v>
       </c>
@@ -4122,7 +4117,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>3</v>
       </c>
@@ -4157,7 +4152,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>3</v>
       </c>
@@ -4192,7 +4187,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>3</v>
       </c>
@@ -4227,7 +4222,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>3</v>
       </c>
@@ -4262,7 +4257,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>3</v>
       </c>
@@ -4297,7 +4292,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>3</v>
       </c>
@@ -4332,7 +4327,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>3</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>3</v>
       </c>
@@ -4402,7 +4397,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>3</v>
       </c>
@@ -4437,7 +4432,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>3</v>
       </c>
@@ -4472,7 +4467,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>3</v>
       </c>
@@ -4507,7 +4502,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>4</v>
       </c>
@@ -4542,7 +4537,7 @@
         <v>2755</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>4</v>
       </c>
@@ -4577,7 +4572,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>4</v>
       </c>
@@ -4612,7 +4607,7 @@
         <v>2355</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>4</v>
       </c>
@@ -4647,7 +4642,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>4</v>
       </c>
@@ -4682,7 +4677,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>4</v>
       </c>
@@ -4717,7 +4712,7 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>4</v>
       </c>
@@ -4752,7 +4747,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>4</v>
       </c>
@@ -4787,7 +4782,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>4</v>
       </c>
@@ -4822,7 +4817,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>4</v>
       </c>
@@ -4857,7 +4852,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>4</v>
       </c>
@@ -4892,7 +4887,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>4</v>
       </c>
@@ -4927,7 +4922,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>4</v>
       </c>
@@ -4962,7 +4957,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>4</v>
       </c>
@@ -4997,7 +4992,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>4</v>
       </c>
@@ -5032,7 +5027,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>4</v>
       </c>
@@ -5067,7 +5062,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>5</v>
       </c>
@@ -5102,7 +5097,7 @@
         <v>5164</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>5</v>
       </c>
@@ -5137,7 +5132,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>5</v>
       </c>
@@ -5172,7 +5167,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>5</v>
       </c>
@@ -5207,7 +5202,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>5</v>
       </c>
@@ -5242,7 +5237,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>5</v>
       </c>
@@ -5277,7 +5272,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>5</v>
       </c>
@@ -5312,7 +5307,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <v>5</v>
       </c>
@@ -5347,7 +5342,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <v>5</v>
       </c>
@@ -5382,7 +5377,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <v>5</v>
       </c>
@@ -5417,7 +5412,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>5</v>
       </c>
@@ -5452,7 +5447,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <v>5</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <v>5</v>
       </c>
@@ -5522,7 +5517,7 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>5</v>
       </c>
@@ -5557,7 +5552,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <v>6</v>
       </c>
@@ -5592,7 +5587,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
         <v>6</v>
       </c>
@@ -5627,7 +5622,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
         <v>6</v>
       </c>
@@ -5662,7 +5657,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
         <v>6</v>
       </c>
@@ -5697,7 +5692,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <v>6</v>
       </c>
@@ -5732,7 +5727,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
         <v>6</v>
       </c>
@@ -5767,7 +5762,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
         <v>6</v>
       </c>
@@ -5802,7 +5797,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <v>6</v>
       </c>
@@ -5837,7 +5832,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <v>6</v>
       </c>
@@ -5872,7 +5867,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <v>6</v>
       </c>
@@ -5907,7 +5902,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
         <v>6</v>
       </c>
@@ -5942,7 +5937,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="8">
         <v>6</v>
       </c>
@@ -5977,7 +5972,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <v>6</v>
       </c>
@@ -6012,7 +6007,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <v>6</v>
       </c>
@@ -6047,7 +6042,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="8">
         <v>7</v>
       </c>
@@ -6082,7 +6077,7 @@
         <v>2682</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="8">
         <v>7</v>
       </c>
@@ -6117,7 +6112,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <v>7</v>
       </c>
@@ -6152,7 +6147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>7</v>
       </c>
@@ -6187,7 +6182,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>7</v>
       </c>
@@ -6222,7 +6217,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <v>7</v>
       </c>
@@ -6257,7 +6252,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <v>7</v>
       </c>
@@ -6292,7 +6287,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>7</v>
       </c>
@@ -6327,7 +6322,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>7</v>
       </c>
@@ -6362,7 +6357,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <v>7</v>
       </c>
@@ -6397,7 +6392,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>7</v>
       </c>
@@ -6432,7 +6427,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
         <v>7</v>
       </c>
@@ -6467,7 +6462,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="8">
         <v>7</v>
       </c>
@@ -6502,7 +6497,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <v>7</v>
       </c>
@@ -6537,7 +6532,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="8">
         <v>7</v>
       </c>
@@ -6572,7 +6567,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
         <v>7</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <v>7</v>
       </c>
@@ -6642,7 +6637,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <v>7</v>
       </c>
@@ -6677,7 +6672,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <v>7</v>
       </c>
@@ -6712,7 +6707,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>8</v>
       </c>
@@ -6747,7 +6742,7 @@
         <v>4093</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <v>8</v>
       </c>
@@ -6782,7 +6777,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <v>8</v>
       </c>
@@ -6817,7 +6812,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="8">
         <v>8</v>
       </c>
@@ -6852,7 +6847,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
         <v>8</v>
       </c>
@@ -6887,7 +6882,7 @@
         <v>3269</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="8">
         <v>8</v>
       </c>
@@ -6922,7 +6917,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <v>8</v>
       </c>
@@ -6957,7 +6952,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <v>8</v>
       </c>
@@ -6992,7 +6987,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <v>9</v>
       </c>
@@ -7027,7 +7022,7 @@
         <v>5905</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="8">
         <v>9</v>
       </c>
@@ -7062,7 +7057,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <v>9</v>
       </c>
@@ -7097,7 +7092,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="8">
         <v>9</v>
       </c>
@@ -7132,7 +7127,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>9</v>
       </c>
@@ -7167,7 +7162,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="8">
         <v>9</v>
       </c>
@@ -7202,7 +7197,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <v>9</v>
       </c>
@@ -7237,7 +7232,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="8">
         <v>9</v>
       </c>
@@ -7272,7 +7267,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="8">
         <v>9</v>
       </c>
@@ -7307,7 +7302,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <v>9</v>
       </c>
@@ -7342,7 +7337,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <v>9</v>
       </c>
@@ -7377,7 +7372,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="8">
         <v>9</v>
       </c>
@@ -7412,7 +7407,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <v>9</v>
       </c>
@@ -7447,7 +7442,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <v>9</v>
       </c>
@@ -7482,7 +7477,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>9</v>
       </c>
@@ -7517,7 +7512,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <v>9</v>
       </c>
@@ -7552,7 +7547,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="8">
         <v>9</v>
       </c>
@@ -7587,7 +7582,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <v>9</v>
       </c>
@@ -7622,7 +7617,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="8">
         <v>9</v>
       </c>
@@ -7657,7 +7652,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>9</v>
       </c>
@@ -7692,7 +7687,7 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <v>9</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>9</v>
       </c>
@@ -7762,7 +7757,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>9</v>
       </c>
@@ -7797,7 +7792,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>9</v>
       </c>
@@ -7832,7 +7827,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>10</v>
       </c>
@@ -7867,7 +7862,7 @@
         <v>2805</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>10</v>
       </c>
@@ -7902,7 +7897,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>10</v>
       </c>
@@ -7937,7 +7932,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>10</v>
       </c>
@@ -7972,7 +7967,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>10</v>
       </c>
@@ -8007,7 +8002,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>10</v>
       </c>
@@ -8042,7 +8037,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>10</v>
       </c>
@@ -8077,7 +8072,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>10</v>
       </c>
@@ -8112,7 +8107,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>10</v>
       </c>
@@ -8147,7 +8142,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <v>10</v>
       </c>
@@ -8182,7 +8177,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <v>10</v>
       </c>
@@ -8217,7 +8212,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>10</v>
       </c>
@@ -8252,7 +8247,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <v>10</v>
       </c>
@@ -8287,7 +8282,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="8">
         <v>10</v>
       </c>
@@ -8322,7 +8317,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="8">
         <v>10</v>
       </c>
@@ -8357,7 +8352,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="8">
         <v>10</v>
       </c>
@@ -8392,7 +8387,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="8">
         <v>10</v>
       </c>
@@ -8427,7 +8422,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="8">
         <v>10</v>
       </c>
@@ -8462,7 +8457,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="8">
         <v>10</v>
       </c>
@@ -8497,7 +8492,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="8">
         <v>10</v>
       </c>
@@ -8532,7 +8527,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <v>10</v>
       </c>
@@ -8567,7 +8562,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="8">
         <v>11</v>
       </c>
@@ -8602,7 +8597,7 @@
         <v>3279</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <v>11</v>
       </c>
@@ -8637,7 +8632,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="8">
         <v>11</v>
       </c>
@@ -8672,7 +8667,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <v>11</v>
       </c>
@@ -8707,7 +8702,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="8">
         <v>11</v>
       </c>
@@ -8742,7 +8737,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="8">
         <v>11</v>
       </c>
@@ -8777,7 +8772,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="8">
         <v>11</v>
       </c>
@@ -8812,7 +8807,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="8">
         <v>11</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="8">
         <v>11</v>
       </c>
@@ -8882,7 +8877,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="8">
         <v>12</v>
       </c>
@@ -8917,7 +8912,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="8">
         <v>12</v>
       </c>
@@ -8952,7 +8947,7 @@
         <v>2488</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="8">
         <v>12</v>
       </c>
@@ -8987,7 +8982,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="8">
         <v>12</v>
       </c>
@@ -9022,7 +9017,7 @@
         <v>1702</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="8">
         <v>12</v>
       </c>
@@ -9057,7 +9052,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="8">
         <v>12</v>
       </c>
@@ -9092,7 +9087,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" s="8">
         <v>12</v>
       </c>
@@ -9127,7 +9122,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" s="8">
         <v>12</v>
       </c>
@@ -9162,7 +9157,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" s="8">
         <v>12</v>
       </c>
@@ -9197,7 +9192,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" s="8">
         <v>12</v>
       </c>
@@ -9232,7 +9227,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <v>12</v>
       </c>
@@ -9267,7 +9262,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" s="8">
         <v>12</v>
       </c>
@@ -9302,7 +9297,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" s="8">
         <v>12</v>
       </c>
@@ -9337,7 +9332,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="8">
         <v>12</v>
       </c>
@@ -9372,7 +9367,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="8">
         <v>12</v>
       </c>
@@ -9407,7 +9402,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" s="8">
         <v>12</v>
       </c>
@@ -9442,7 +9437,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" s="8">
         <v>12</v>
       </c>
@@ -9477,7 +9472,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" s="8">
         <v>12</v>
       </c>
@@ -9512,7 +9507,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" s="8">
         <v>12</v>
       </c>
@@ -9547,7 +9542,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" s="8">
         <v>12</v>
       </c>
@@ -9582,7 +9577,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" s="8">
         <v>12</v>
       </c>
@@ -9617,7 +9612,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" s="8">
         <v>12</v>
       </c>
@@ -9652,7 +9647,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="8">
         <v>12</v>
       </c>
@@ -9687,7 +9682,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="8">
         <v>12</v>
       </c>
@@ -9722,7 +9717,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="8">
         <v>12</v>
       </c>
@@ -9757,7 +9752,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" s="8">
         <v>12</v>
       </c>
@@ -9792,7 +9787,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="8">
         <v>12</v>
       </c>
@@ -9827,7 +9822,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="8">
         <v>12</v>
       </c>
@@ -9862,7 +9857,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="8">
         <v>12</v>
       </c>
@@ -9897,7 +9892,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" s="8">
         <v>12</v>
       </c>
@@ -9932,7 +9927,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" s="8">
         <v>13</v>
       </c>
@@ -9967,7 +9962,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" s="8">
         <v>13</v>
       </c>
@@ -10002,7 +9997,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" s="8">
         <v>13</v>
       </c>
@@ -10037,7 +10032,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" s="8">
         <v>13</v>
       </c>
@@ -10072,7 +10067,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A205" s="8">
         <v>13</v>
       </c>
@@ -10107,7 +10102,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" s="8">
         <v>13</v>
       </c>
@@ -10142,7 +10137,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" s="8">
         <v>13</v>
       </c>
@@ -10177,7 +10172,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" s="8">
         <v>13</v>
       </c>
@@ -10212,7 +10207,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" s="8">
         <v>13</v>
       </c>
@@ -10247,7 +10242,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A210" s="8">
         <v>13</v>
       </c>
@@ -10282,7 +10277,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A211" s="8">
         <v>13</v>
       </c>
@@ -10317,7 +10312,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A212" s="8">
         <v>13</v>
       </c>
@@ -10352,7 +10347,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A213" s="8">
         <v>13</v>
       </c>
@@ -10387,7 +10382,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A214" s="8">
         <v>13</v>
       </c>
@@ -10422,7 +10417,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" s="8">
         <v>13</v>
       </c>
@@ -10457,7 +10452,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A216" s="8">
         <v>13</v>
       </c>
@@ -10492,7 +10487,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A217" s="8">
         <v>13</v>
       </c>
@@ -10527,7 +10522,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A218" s="8">
         <v>13</v>
       </c>
@@ -10562,7 +10557,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A219" s="8">
         <v>13</v>
       </c>
@@ -10597,7 +10592,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A220" s="8">
         <v>13</v>
       </c>
@@ -10632,7 +10627,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A221" s="8">
         <v>13</v>
       </c>
@@ -10667,7 +10662,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A222" s="8">
         <v>13</v>
       </c>
@@ -10702,7 +10697,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A223" s="8">
         <v>13</v>
       </c>
@@ -10737,7 +10732,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A224" s="8">
         <v>13</v>
       </c>
@@ -10772,7 +10767,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A225" s="8">
         <v>13</v>
       </c>
@@ -10807,7 +10802,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A226" s="8">
         <v>13</v>
       </c>
@@ -10842,7 +10837,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A227" s="8">
         <v>13</v>
       </c>
@@ -10877,7 +10872,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" s="8">
         <v>13</v>
       </c>
@@ -10912,7 +10907,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" s="8">
         <v>13</v>
       </c>
@@ -10947,7 +10942,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" s="8">
         <v>13</v>
       </c>
@@ -10982,7 +10977,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A231" s="8">
         <v>13</v>
       </c>
@@ -11017,7 +11012,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A232" s="8">
         <v>13</v>
       </c>
@@ -11052,7 +11047,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A233" s="8">
         <v>13</v>
       </c>
@@ -11087,7 +11082,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A234" s="8">
         <v>14</v>
       </c>
@@ -11122,7 +11117,7 @@
         <v>2959</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" s="8">
         <v>14</v>
       </c>
@@ -11157,7 +11152,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A236" s="8">
         <v>14</v>
       </c>
@@ -11192,7 +11187,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A237" s="8">
         <v>14</v>
       </c>
@@ -11227,7 +11222,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" s="8">
         <v>14</v>
       </c>
@@ -11262,7 +11257,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" s="8">
         <v>14</v>
       </c>
@@ -11297,7 +11292,7 @@
         <v>3877</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" s="8">
         <v>14</v>
       </c>
@@ -11332,7 +11327,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" s="8">
         <v>14</v>
       </c>
@@ -11367,7 +11362,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" s="8">
         <v>14</v>
       </c>
@@ -11402,7 +11397,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" s="8">
         <v>14</v>
       </c>
@@ -11437,7 +11432,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" s="8">
         <v>14</v>
       </c>
@@ -11472,7 +11467,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" s="8">
         <v>14</v>
       </c>
@@ -11507,7 +11502,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" s="8">
         <v>14</v>
       </c>
@@ -11542,7 +11537,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" s="8">
         <v>14</v>
       </c>
@@ -11577,7 +11572,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" s="8">
         <v>14</v>
       </c>
@@ -11612,7 +11607,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" s="8">
         <v>14</v>
       </c>
@@ -11647,7 +11642,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" s="8">
         <v>14</v>
       </c>
@@ -11682,7 +11677,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" s="8">
         <v>14</v>
       </c>
@@ -11717,7 +11712,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" s="8">
         <v>14</v>
       </c>
@@ -11752,7 +11747,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A253" s="8">
         <v>14</v>
       </c>
@@ -11787,7 +11782,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" s="8">
         <v>14</v>
       </c>
@@ -11822,7 +11817,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" s="8">
         <v>15</v>
       </c>
@@ -11857,7 +11852,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" s="8">
         <v>15</v>
       </c>
@@ -11892,7 +11887,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" s="8">
         <v>15</v>
       </c>
@@ -11927,7 +11922,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" s="8">
         <v>15</v>
       </c>
@@ -11962,7 +11957,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" s="8">
         <v>15</v>
       </c>
@@ -11997,7 +11992,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" s="8">
         <v>15</v>
       </c>
@@ -12032,7 +12027,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" s="8">
         <v>15</v>
       </c>
@@ -12067,7 +12062,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A262" s="8">
         <v>15</v>
       </c>
@@ -12102,7 +12097,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" s="8">
         <v>16</v>
       </c>
@@ -12137,7 +12132,7 @@
         <v>4818</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" s="8">
         <v>16</v>
       </c>
@@ -12172,7 +12167,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" s="8">
         <v>16</v>
       </c>
@@ -12207,7 +12202,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" s="8">
         <v>16</v>
       </c>
@@ -12242,7 +12237,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" s="8">
         <v>16</v>
       </c>
@@ -12277,7 +12272,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" s="8">
         <v>16</v>
       </c>
@@ -12312,7 +12307,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" s="8">
         <v>16</v>
       </c>
@@ -12347,7 +12342,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A270" s="8">
         <v>16</v>
       </c>
@@ -12382,7 +12377,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" s="8">
         <v>16</v>
       </c>
@@ -12417,7 +12412,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" s="8">
         <v>16</v>
       </c>
@@ -12452,7 +12447,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" s="8">
         <v>16</v>
       </c>
@@ -12487,7 +12482,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" s="8">
         <v>16</v>
       </c>
@@ -12522,7 +12517,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" s="8">
         <v>16</v>
       </c>
@@ -12557,7 +12552,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" s="8">
         <v>16</v>
       </c>
@@ -12592,7 +12587,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" s="8">
         <v>16</v>
       </c>
@@ -12627,7 +12622,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" s="8">
         <v>16</v>
       </c>
@@ -12662,7 +12657,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" s="8">
         <v>16</v>
       </c>
@@ -12697,7 +12692,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" s="8">
         <v>17</v>
       </c>
@@ -12732,7 +12727,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" s="8">
         <v>17</v>
       </c>
@@ -12767,7 +12762,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" s="8">
         <v>17</v>
       </c>
@@ -12802,7 +12797,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" s="8">
         <v>17</v>
       </c>
@@ -12837,7 +12832,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" s="8">
         <v>17</v>
       </c>
@@ -12872,7 +12867,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" s="8">
         <v>17</v>
       </c>
@@ -12907,7 +12902,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" s="8">
         <v>17</v>
       </c>
@@ -12942,7 +12937,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" s="8">
         <v>17</v>
       </c>
@@ -12977,7 +12972,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" s="8">
         <v>17</v>
       </c>
@@ -13012,7 +13007,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" s="8">
         <v>17</v>
       </c>
@@ -13047,7 +13042,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" s="8">
         <v>17</v>
       </c>
@@ -13082,7 +13077,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" s="8">
         <v>17</v>
       </c>
@@ -13117,7 +13112,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" s="8">
         <v>17</v>
       </c>
@@ -13152,7 +13147,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" s="8">
         <v>17</v>
       </c>
@@ -13187,7 +13182,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" s="8">
         <v>18</v>
       </c>
@@ -13222,7 +13217,7 @@
         <v>3252</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" s="8">
         <v>18</v>
       </c>
@@ -13257,7 +13252,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" s="8">
         <v>18</v>
       </c>
@@ -13292,7 +13287,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" s="8">
         <v>18</v>
       </c>
@@ -13327,7 +13322,7 @@
         <v>3249</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" s="8">
         <v>18</v>
       </c>
@@ -13362,7 +13357,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" s="8">
         <v>19</v>
       </c>
@@ -13397,7 +13392,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" s="8">
         <v>19</v>
       </c>
@@ -13432,7 +13427,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" s="8">
         <v>19</v>
       </c>
@@ -13467,7 +13462,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" s="8">
         <v>19</v>
       </c>
@@ -13502,7 +13497,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" s="8">
         <v>19</v>
       </c>
@@ -13537,7 +13532,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" s="8">
         <v>19</v>
       </c>
@@ -13572,7 +13567,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" s="8">
         <v>19</v>
       </c>
@@ -13607,7 +13602,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" s="8">
         <v>19</v>
       </c>
@@ -13642,7 +13637,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" s="8">
         <v>19</v>
       </c>
@@ -13677,7 +13672,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" s="8">
         <v>19</v>
       </c>
@@ -13712,7 +13707,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" s="8">
         <v>19</v>
       </c>
@@ -13747,7 +13742,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" s="8">
         <v>20</v>
       </c>
@@ -13782,7 +13777,7 @@
         <v>3812</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" s="8">
         <v>20</v>
       </c>
@@ -13817,7 +13812,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" s="8">
         <v>20</v>
       </c>
@@ -13852,7 +13847,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" s="8">
         <v>20</v>
       </c>
@@ -13887,7 +13882,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" s="8">
         <v>20</v>
       </c>
@@ -13922,7 +13917,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" s="8">
         <v>20</v>
       </c>
@@ -13957,7 +13952,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" s="8">
         <v>20</v>
       </c>
@@ -13992,7 +13987,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" s="8">
         <v>20</v>
       </c>
@@ -14027,7 +14022,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" s="8">
         <v>20</v>
       </c>
@@ -14062,7 +14057,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" s="8">
         <v>20</v>
       </c>
@@ -14097,7 +14092,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" s="8">
         <v>20</v>
       </c>
@@ -14132,7 +14127,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" s="8">
         <v>21</v>
       </c>
@@ -14167,7 +14162,7 @@
         <v>4807</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" s="8">
         <v>21</v>
       </c>
@@ -14202,7 +14197,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A323" s="8">
         <v>21</v>
       </c>
@@ -14237,7 +14232,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A324" s="8">
         <v>21</v>
       </c>
@@ -14272,7 +14267,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A325" s="8">
         <v>21</v>
       </c>
@@ -14307,7 +14302,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A326" s="8">
         <v>21</v>
       </c>
@@ -14342,7 +14337,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A327" s="8">
         <v>21</v>
       </c>
@@ -14377,7 +14372,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A328" s="8">
         <v>22</v>
       </c>
@@ -14412,7 +14407,7 @@
         <v>4790</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A329" s="8">
         <v>22</v>
       </c>
@@ -14447,7 +14442,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A330" s="8">
         <v>22</v>
       </c>
@@ -14482,7 +14477,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A331" s="8">
         <v>22</v>
       </c>
@@ -14517,7 +14512,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" s="8">
         <v>22</v>
       </c>
@@ -14552,7 +14547,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A333" s="8">
         <v>22</v>
       </c>
@@ -14587,7 +14582,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A334" s="8">
         <v>22</v>
       </c>
@@ -14622,7 +14617,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A335" s="8">
         <v>22</v>
       </c>
@@ -14657,7 +14652,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A336" s="8">
         <v>22</v>
       </c>
@@ -14692,7 +14687,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A337" s="8">
         <v>22</v>
       </c>
@@ -14727,7 +14722,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A338" s="8">
         <v>22</v>
       </c>
@@ -14762,7 +14757,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" s="8">
         <v>22</v>
       </c>
@@ -14797,7 +14792,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" s="8">
         <v>22</v>
       </c>
@@ -14832,7 +14827,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" s="8">
         <v>22</v>
       </c>
@@ -14867,7 +14862,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A342" s="8">
         <v>22</v>
       </c>
@@ -14902,7 +14897,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A343" s="8">
         <v>22</v>
       </c>
@@ -14937,7 +14932,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A344" s="20">
         <v>22</v>
       </c>
@@ -14972,24 +14967,24 @@
         <v>883</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A345" s="43"/>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A345" s="40"/>
       <c r="B345" s="9"/>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A346" s="43" t="s">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A346" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B346" s="44"/>
-      <c r="C346" s="45"/>
+      <c r="B346" s="41"/>
+      <c r="C346" s="42"/>
       <c r="D346" s="33"/>
-      <c r="E346" s="46"/>
-      <c r="F346" s="46"/>
-      <c r="G346" s="46"/>
-      <c r="H346" s="46"/>
-      <c r="I346" s="46"/>
-      <c r="J346" s="46"/>
-      <c r="K346" s="46"/>
+      <c r="E346" s="43"/>
+      <c r="F346" s="43"/>
+      <c r="G346" s="43"/>
+      <c r="H346" s="43"/>
+      <c r="I346" s="43"/>
+      <c r="J346" s="43"/>
+      <c r="K346" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>